<commit_message>
Found some bugs and inconsistancies retesting the registration process, this commit has fixes for them
</commit_message>
<xml_diff>
--- a/requirements_matrix.xlsx
+++ b/requirements_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megan/Development/Portfolio/contact-manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DC523C-7A59-4F45-A5F6-4B5DCB94A083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD2A0DE-316B-C34C-A82F-FEB43BCBC695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="15500" xr2:uid="{A8F6B397-6B0C-C04E-8135-E26AF54F279C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="95">
   <si>
     <t>General Requirements</t>
   </si>
@@ -633,9 +633,6 @@
       </rPr>
       <t>/delete"</t>
     </r>
-  </si>
-  <si>
-    <t>Similar folder layout, called the database interface connections-db rather than pg-persistence</t>
   </si>
   <si>
     <t>The application must not be one of the projects from either JS175 or JS185, nor may it be a closely related application. For instance, a TodoList application would not be appropriate even if it provides behaviors not supported by the JS175/JS185 versions.</t>
@@ -1203,10 +1200,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> - Pagination for contacts and objectives redirects and provides an appropriate message if invalid page is requested.
- - </t>
-  </si>
-  <si>
     <t xml:space="preserve">Validation errors from 2.7 are delivered as described in 2.8 using flash. Error messages are hand tailored and encompass checks mirroring browser delivered validation in case user bypasses the browser through postman or curl. </t>
   </si>
   <si>
@@ -1219,6 +1212,22 @@
 Objectives are sorted by occasion</t>
   </si>
   <si>
+    <t xml:space="preserve">Error messages are presented on the same page for user input validation. 
+For the most part even invalid data is preserved. Personally, I find it helpful to be able to see what I did that was rejected. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I built up the application registration/account access process to give myself a little more pug-express-sql practice before jumping into the meat and potatoes of the application and to feel more confident with the concept of session management. I didn't want to just copy-paste-edit the todo app, I thought I would get more out of a ground up build. But, I did stop at the user/home page. That page is there as a placeholder and is intended to be the presentation page for the data entered through the contacts and objectives page. </t>
+  </si>
+  <si>
+    <t>An application home page provided details as to the application's intent</t>
+  </si>
+  <si>
+    <t>The route hierarchy was established with organizational intent</t>
+  </si>
+  <si>
+    <t>Each creation, update and delete of a contact or an objective is reflected in the database</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1306,8 +1315,9 @@
       </rPr>
       <t xml:space="preserve">:  I require no more than a name concatenation to be truthy for a contact to have sufficient data to be stored. These fields are mainly present for user reference, it's basically a rolodex. This looseness of data actually made it harder to validate, because the logic was- you can be empty, but if you aren't, make sure your data is of valid format. The checks that were made are generally of format:
     - trim, 
+    - allow for empty provision
     - vet to avoid triggering a failure on the SQL INSERT/UPDATE statement
-    - check for proper format from a use perspective 
+    - check for proper format from a functional perspective 
     - </t>
     </r>
     <r>
@@ -1355,12 +1365,58 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Error messages are presented on the same page for user input validation. 
-For the most part even invalid data is preserved. Personally, I find it helpful to be able to see what I did that was rejected. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">There are two functions that are intended to manage accessibility. 
+    <r>
+      <t xml:space="preserve"> - Pagination for contacts and objectives redirects and provides an appropriate message if invalid page is requested. (There are tests for this documentes under requirment 2.5.2)
+ - Created two functions to authenticate contact-id and objectove-id enabled access
+    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>requiresUserContactValidation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: if a signed in user attempts to access a contact which does not belong to them, this function will redirect them to their contacts page with a flash error
+    - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>requiresContactObjectiveValidation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: if a signed in user attempts to access a conective they own through the wrong contact, this function will redirect them to their specified contact-id page with a flash error. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There are two functions that are intended to manage accessibility.
 - </t>
     </r>
     <r>
@@ -1382,7 +1438,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: checks for signin and reroutes any requests trying to access a /user... extension to /login if a signin is false.
+      <t xml:space="preserve">: checks for signin and reroutes any requests trying to access a /user... extension to /the application home page which has a login tab if a signin is false.
 - </t>
     </r>
     <r>
@@ -1404,25 +1460,57 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">: 
-There exist two routes which do not invoke one of these two checks, the application home page (/home), this is intended to be public, and the instruction sub page (/home/how-it-works), this is also intended to be public. 
+      <t xml:space="preserve">: This function redirects a logged in user from the login page to the user/home. a logged in user doens't need to log in.
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>public pages:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> There exist two routes which do not invoke one of these two checks, the application home page (/home), this is intended to be public, and the instruction sub page (/home/how-it-works), this is also intended to be public. 
 </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">I built up the application registration/account access process to give myself a little more pug-express-sql practice before jumping into the meat and potatoes of the application and to feel more confident with the concept of session management. I didn't want to just copy-paste-edit the todo app, I thought I would get more out of a ground up build. But, I did stop at the user/home page. That page is there as a placeholder and is intended to be the presentation page for the data entered through the contacts and objectives page. </t>
-  </si>
-  <si>
-    <t>An application home page provided details as to the application's intent</t>
-  </si>
-  <si>
-    <t>The route hierarchy was established with organizational intent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This application has been on my todo-list for awhile. I jumped right into it for this project and didn't even remember until I was double checking validation that we had technically made a "contact-manager" in 175. There was zero information used from that set of code, it wasn't referenced, in fact I didn't even remember it existed before I stumbled across it in validation checking. They are not similar beyond sharing a domain space. </t>
-  </si>
-  <si>
-    <t>Each creation, update and delete of a contact or an objective is reflected in the database</t>
+    <t>Application Specific Requirements 2.1 to 2.11 have been met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar folder layout, called the database interface connections-db rather than pg-persistence. I do have two layouts view templates, one top layer, the other nested into the user directory. I set it up to be able to cascade views into the user directory, but didn't end up utilizing the feature. RIght now that second layout is more of an empty conduit. </t>
+  </si>
+  <si>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Database files
+- schema.sql
+- lib/data/
+    - seed-data.sql
+    - contacts.sql
+    - objectives.sql
+    - create-connections-db.sh
+    - load-schema.sh
+    - load-contacts.sh
+    - load-objectives.sh
+To populate the database, execute  create-connections-db.sh, then load-schema.sh, then load-contacts.sh, then load-objectives.sh from the data directory. The first file will delete any existing connections database, than create a new one. The second file will load the schema and the user data. The third file will load contacts, the fourth file will load objectives.
+The resulting database will have 3 profiles: admin, developer, and user. The corresponding passwords are adminPass, developerPass, and userPass. The admin account will have 100 randomly generated contacts with 1000 randomly generated connections. The other two accounts will be empty.</t>
+  </si>
+  <si>
+    <t>This application has been on my todo-list for awhile. I jumped right into it for this project and didn't even remember until I was double checking validation that we had technically made a "contact-manager" in 175. There was zero information used from that set of code to build this application, it wasn't referenced, in fact I didn't even remember it existed before I stumbled across it in validation checking. They are not similar beyond sharing a domain space. I do believe I satisfied the spirit of this requirement.</t>
   </si>
 </sst>
 </file>
@@ -1891,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7A6783-E2E8-204A-BB4F-E6E76C2B8B65}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" outlineLevelRow="1"/>
@@ -1915,7 +2003,7 @@
         <v>28</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="22">
@@ -1926,7 +2014,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="22" hidden="1" outlineLevel="1">
@@ -1984,15 +2072,18 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" collapsed="1">
-      <c r="A8" s="3">
+    <row r="8" spans="1:4" ht="22" collapsed="1">
+      <c r="A8" s="4">
         <v>2</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="87">
+      <c r="C8" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="87" hidden="1" outlineLevel="1">
       <c r="A9" s="4">
         <v>2.1</v>
       </c>
@@ -2003,7 +2094,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="176">
+    <row r="10" spans="1:4" ht="176" hidden="1" outlineLevel="1">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -2011,19 +2102,19 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="44">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="44" hidden="1" outlineLevel="1">
       <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="409.6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="409.6" hidden="1" outlineLevel="1">
       <c r="A12" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2031,10 +2122,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="44">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="44" hidden="1" outlineLevel="1">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -2042,13 +2133,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="42">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="42" hidden="1" outlineLevel="1">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2150,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="44">
+    <row r="15" spans="1:4" ht="44" hidden="1" outlineLevel="1">
       <c r="A15" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2067,13 +2158,13 @@
         <v>10</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="111">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="111" hidden="1" outlineLevel="1">
       <c r="A16" s="4">
         <v>2.4</v>
       </c>
@@ -2084,7 +2175,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="106">
+    <row r="17" spans="1:4" ht="106" hidden="1" outlineLevel="1">
       <c r="A17" s="4">
         <v>2.5</v>
       </c>
@@ -2092,19 +2183,19 @@
         <v>33</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="154">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="154" hidden="1" outlineLevel="1">
       <c r="A18" s="4"/>
       <c r="B18" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="63">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="63" hidden="1" outlineLevel="1">
       <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
@@ -2112,13 +2203,13 @@
         <v>12</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="154">
+    </row>
+    <row r="20" spans="1:4" ht="154" hidden="1" outlineLevel="1">
       <c r="A20" s="4">
         <v>2.6</v>
       </c>
@@ -2126,10 +2217,10 @@
         <v>13</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="409.6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="409.6" hidden="1" outlineLevel="1">
       <c r="A21" s="4">
         <v>2.7</v>
       </c>
@@ -2137,10 +2228,10 @@
         <v>14</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="88" hidden="1" outlineLevel="1">
       <c r="A22" s="4">
         <v>2.8</v>
       </c>
@@ -2148,10 +2239,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="66">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="66" hidden="1" outlineLevel="1">
       <c r="A23" s="4">
         <v>2.9</v>
       </c>
@@ -2159,32 +2250,32 @@
         <v>16</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="66">
-      <c r="A24" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="264" hidden="1" outlineLevel="1">
+      <c r="A24" s="4">
         <v>2.1</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="176">
-      <c r="A25" s="10">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="286" hidden="1" outlineLevel="1">
+      <c r="A25" s="4">
         <v>2.11</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" collapsed="1">
       <c r="A26" s="3">
         <v>3</v>
       </c>
@@ -2193,57 +2284,69 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="154">
-      <c r="A27" s="10">
+      <c r="A27" s="4">
         <v>3.1</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="44">
-      <c r="A28" s="10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="110">
+      <c r="A28" s="4">
         <v>3.2</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="48">
-      <c r="A29" s="10">
+      <c r="A29" s="4">
         <v>3.3</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="63">
-      <c r="A30" s="10">
+      <c r="C29" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="409.6">
+      <c r="A30" s="4">
         <v>3.4</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="C30" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="48">
-      <c r="A31" s="10">
+      <c r="A31" s="4">
         <v>3.5</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>36</v>
       </c>
+      <c r="C31" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="111">
-      <c r="A32" s="3">
+      <c r="A32" s="4">
         <v>3.6</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>37</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="24">
@@ -2294,7 +2397,7 @@
         <v>26</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="22">
@@ -2305,18 +2408,18 @@
         <v>27</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="132">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="154">
       <c r="A40" s="4">
         <v>4</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2364,10 +2467,10 @@
         <v>52</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="15"/>
     </row>
@@ -2376,10 +2479,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="409.6">
@@ -2387,10 +2490,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="409.6">
@@ -2398,10 +2501,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>78</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>

<commit_message>
completed reqirements matrix, and home page text, updated css fro detailed contacts
</commit_message>
<xml_diff>
--- a/requirements_matrix.xlsx
+++ b/requirements_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megan/Development/Portfolio/contact-manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD2A0DE-316B-C34C-A82F-FEB43BCBC695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84654D2-8C56-8B40-AFDD-34E53896C87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="15500" xr2:uid="{A8F6B397-6B0C-C04E-8135-E26AF54F279C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
   <si>
     <t>General Requirements</t>
   </si>
@@ -1496,21 +1496,24 @@
     <t>check</t>
   </si>
   <si>
+    <t>This application has been on my todo-list for awhile. I jumped right into it for this project and didn't even remember until I was double checking validation that we had technically made a "contact-manager" in 175. There was zero information used from that set of code to build this application, it wasn't referenced, in fact I didn't even remember it existed before I stumbled across it in validation checking. They are not similar beyond sharing a domain space. I do believe I satisfied the spirit of this requirement.</t>
+  </si>
+  <si>
     <t>Database files
 - schema.sql
 - lib/data/
-    - seed-data.sql
+    - users.sql
     - contacts.sql
     - objectives.sql
     - create-connections-db.sh
-    - load-schema.sh
+    - load-users.sh
     - load-contacts.sh
     - load-objectives.sh
 To populate the database, execute  create-connections-db.sh, then load-schema.sh, then load-contacts.sh, then load-objectives.sh from the data directory. The first file will delete any existing connections database, than create a new one. The second file will load the schema and the user data. The third file will load contacts, the fourth file will load objectives.
 The resulting database will have 3 profiles: admin, developer, and user. The corresponding passwords are adminPass, developerPass, and userPass. The admin account will have 100 randomly generated contacts with 1000 randomly generated connections. The other two accounts will be empty.</t>
   </si>
   <si>
-    <t>This application has been on my todo-list for awhile. I jumped right into it for this project and didn't even remember until I was double checking validation that we had technically made a "contact-manager" in 175. There was zero information used from that set of code to build this application, it wasn't referenced, in fact I didn't even remember it existed before I stumbled across it in validation checking. They are not similar beyond sharing a domain space. I do believe I satisfied the spirit of this requirement.</t>
+    <t>Other requirements 3.1-3-7 complete</t>
   </si>
 </sst>
 </file>
@@ -1979,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE7A6783-E2E8-204A-BB4F-E6E76C2B8B65}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" outlineLevelRow="1"/>
@@ -2017,7 +2020,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="22" hidden="1" outlineLevel="1">
+    <row r="3" spans="1:4" ht="22" outlineLevel="1">
       <c r="A3" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="22" hidden="1" outlineLevel="1">
+    <row r="4" spans="1:4" ht="22" outlineLevel="1">
       <c r="A4" s="4">
         <v>1.2</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" hidden="1" outlineLevel="1">
+    <row r="5" spans="1:4" ht="45" outlineLevel="1">
       <c r="A5" s="4">
         <v>1.3</v>
       </c>
@@ -2050,7 +2053,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="198" hidden="1" outlineLevel="1">
+    <row r="6" spans="1:4" ht="198" outlineLevel="1">
       <c r="A6" s="4">
         <v>1.4</v>
       </c>
@@ -2061,7 +2064,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="85" hidden="1" outlineLevel="1">
+    <row r="7" spans="1:4" ht="85" outlineLevel="1">
       <c r="A7" s="4">
         <v>1.5</v>
       </c>
@@ -2072,7 +2075,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22" collapsed="1">
+    <row r="8" spans="1:4" ht="22">
       <c r="A8" s="4">
         <v>2</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="87" hidden="1" outlineLevel="1">
+    <row r="9" spans="1:4" ht="87" outlineLevel="1">
       <c r="A9" s="4">
         <v>2.1</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="176" hidden="1" outlineLevel="1">
+    <row r="10" spans="1:4" ht="176" outlineLevel="1">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="44" hidden="1" outlineLevel="1">
+    <row r="11" spans="1:4" ht="44" outlineLevel="1">
       <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
         <v>6</v>
@@ -2114,7 +2117,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="409.6" hidden="1" outlineLevel="1">
+    <row r="12" spans="1:4" ht="409.6" outlineLevel="1">
       <c r="A12" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="44" hidden="1" outlineLevel="1">
+    <row r="13" spans="1:4" ht="44" outlineLevel="1">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="42" hidden="1" outlineLevel="1">
+    <row r="14" spans="1:4" ht="42" outlineLevel="1">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="44" hidden="1" outlineLevel="1">
+    <row r="15" spans="1:4" ht="44" outlineLevel="1">
       <c r="A15" s="4">
         <v>2.2999999999999998</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="111" hidden="1" outlineLevel="1">
+    <row r="16" spans="1:4" ht="111" outlineLevel="1">
       <c r="A16" s="4">
         <v>2.4</v>
       </c>
@@ -2175,7 +2178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="106" hidden="1" outlineLevel="1">
+    <row r="17" spans="1:4" ht="106" outlineLevel="1">
       <c r="A17" s="4">
         <v>2.5</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="154" hidden="1" outlineLevel="1">
+    <row r="18" spans="1:4" ht="154" outlineLevel="1">
       <c r="A18" s="4"/>
       <c r="B18" s="9" t="s">
         <v>11</v>
@@ -2195,7 +2198,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="63" hidden="1" outlineLevel="1">
+    <row r="19" spans="1:4" ht="63" outlineLevel="1">
       <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="154" hidden="1" outlineLevel="1">
+    <row r="20" spans="1:4" ht="154" outlineLevel="1">
       <c r="A20" s="4">
         <v>2.6</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="409.6" hidden="1" outlineLevel="1">
+    <row r="21" spans="1:4" ht="409.6" outlineLevel="1">
       <c r="A21" s="4">
         <v>2.7</v>
       </c>
@@ -2231,7 +2234,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="88" hidden="1" outlineLevel="1">
+    <row r="22" spans="1:4" ht="88" outlineLevel="1">
       <c r="A22" s="4">
         <v>2.8</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="66" hidden="1" outlineLevel="1">
+    <row r="23" spans="1:4" ht="66" outlineLevel="1">
       <c r="A23" s="4">
         <v>2.9</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="264" hidden="1" outlineLevel="1">
+    <row r="24" spans="1:4" ht="264" outlineLevel="1">
       <c r="A24" s="4">
         <v>2.1</v>
       </c>
@@ -2264,7 +2267,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="286" hidden="1" outlineLevel="1">
+    <row r="25" spans="1:4" ht="286" outlineLevel="1">
       <c r="A25" s="4">
         <v>2.11</v>
       </c>
@@ -2275,12 +2278,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:4" collapsed="1">
-      <c r="A26" s="3">
+    <row r="26" spans="1:4" ht="22">
+      <c r="A26" s="4">
         <v>3</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>18</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="154">
@@ -2324,7 +2330,7 @@
         <v>21</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="48">
@@ -2350,43 +2356,58 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="24">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>38</v>
       </c>
+      <c r="C33" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="42">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="3" t="s">
+      <c r="C34" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="22">
+      <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="3" t="s">
+      <c r="C35" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="22">
+      <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="3" t="s">
+      <c r="C36" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="22">
+      <c r="A37" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="63">
@@ -2419,7 +2440,7 @@
         <v>61</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:3">

</xml_diff>